<commit_message>
Accreditamento RSA e LDO SIS4CARE
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/accreditamento-checklist_V8.2.6.1.xlsx
+++ b/GATEWAY/A1#111SIS4CAREXX/POLIS-NET_SRL/SIS4CARE/v1.1.0/accreditamento-checklist_V8.2.6.1.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="592">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2181,7 +2181,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2309,12 +2309,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2525,7 +2519,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2706,15 +2700,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2730,7 +2720,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2738,7 +2728,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2754,7 +2744,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3096,7 +3086,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="N169 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3110,32 +3100,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="285.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3148,12 +3138,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -3183,7 +3173,7 @@
   <dimension ref="A1:B996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="N169 B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4260,11 +4250,11 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B169" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="C126" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
-      <selection pane="bottomRight" activeCell="N169" activeCellId="0" sqref="N169"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A126" activeCellId="0" sqref="A126"/>
+      <selection pane="bottomRight" activeCell="J128" activeCellId="0" sqref="J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4482,7 +4472,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="17"/>
     </row>
-    <row r="9" s="30" customFormat="true" ht="137.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="30" customFormat="true" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
         <v>24</v>
       </c>
@@ -4627,7 +4617,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="n">
         <v>29</v>
       </c>
@@ -4762,7 +4752,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="n">
         <v>32</v>
       </c>
@@ -4813,7 +4803,7 @@
       <c r="R15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="S15" s="47" t="s">
+      <c r="S15" s="37" t="s">
         <v>64</v>
       </c>
       <c r="T15" s="37"/>
@@ -4971,7 +4961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="n">
         <v>37</v>
       </c>
@@ -5069,7 +5059,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="150.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="33" t="n">
         <v>39</v>
       </c>
@@ -5106,7 +5096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="n">
         <v>40</v>
       </c>
@@ -5157,7 +5147,7 @@
       <c r="R23" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="S23" s="47" t="s">
+      <c r="S23" s="37" t="s">
         <v>64</v>
       </c>
       <c r="T23" s="37"/>
@@ -5317,7 +5307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="33" t="n">
         <v>45</v>
       </c>
@@ -5411,7 +5401,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="82.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="33" t="n">
         <v>47</v>
       </c>
@@ -5450,7 +5440,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" s="49" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="48" customFormat="true" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="33" t="n">
         <v>48</v>
       </c>
@@ -5468,7 +5458,7 @@
       </c>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
-      <c r="H31" s="48"/>
+      <c r="H31" s="47"/>
       <c r="I31" s="42"/>
       <c r="J31" s="37" t="s">
         <v>61</v>
@@ -5881,7 +5871,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="120.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="108.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="33" t="n">
         <v>62</v>
       </c>
@@ -5918,7 +5908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="33" t="n">
         <v>64</v>
       </c>
@@ -5979,7 +5969,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="33" t="n">
         <v>66</v>
       </c>
@@ -6040,7 +6030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="33" t="n">
         <v>67</v>
       </c>
@@ -6101,7 +6091,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="33" t="n">
         <v>68</v>
       </c>
@@ -6162,7 +6152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="464.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="391" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="33" t="n">
         <v>69</v>
       </c>
@@ -6201,7 +6191,7 @@
       <c r="N47" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O47" s="50" t="s">
+      <c r="O47" s="49" t="s">
         <v>158</v>
       </c>
       <c r="P47" s="37" t="s">
@@ -6219,7 +6209,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="33" t="n">
         <v>70</v>
       </c>
@@ -6278,7 +6268,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="33" t="n">
         <v>71</v>
       </c>
@@ -6337,7 +6327,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="33" t="n">
         <v>72</v>
       </c>
@@ -6396,7 +6386,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="33" t="n">
         <v>73</v>
       </c>
@@ -6455,7 +6445,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="33" t="n">
         <v>74</v>
       </c>
@@ -8808,7 +8798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="105.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="95.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="33" t="n">
         <v>146</v>
       </c>
@@ -8845,7 +8835,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="116" s="49" customFormat="true" ht="100.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="116" s="48" customFormat="true" ht="100.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="33" t="n">
         <v>152</v>
       </c>
@@ -8870,7 +8860,7 @@
       <c r="H116" s="46" t="s">
         <v>324</v>
       </c>
-      <c r="I116" s="51" t="s">
+      <c r="I116" s="50" t="s">
         <v>325</v>
       </c>
       <c r="J116" s="37" t="s">
@@ -8886,7 +8876,7 @@
       <c r="N116" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O116" s="52" t="s">
+      <c r="O116" s="51" t="s">
         <v>327</v>
       </c>
       <c r="P116" s="37" t="s">
@@ -8908,7 +8898,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="117" s="49" customFormat="true" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" s="48" customFormat="true" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="33" t="n">
         <v>154</v>
       </c>
@@ -8933,7 +8923,7 @@
       <c r="H117" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="I117" s="51" t="s">
+      <c r="I117" s="50" t="s">
         <v>334</v>
       </c>
       <c r="J117" s="37" t="s">
@@ -8949,7 +8939,7 @@
       <c r="N117" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O117" s="53" t="s">
+      <c r="O117" s="52" t="s">
         <v>137</v>
       </c>
       <c r="P117" s="37" t="s">
@@ -8971,7 +8961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="33" t="n">
         <v>155</v>
       </c>
@@ -8993,7 +8983,7 @@
       <c r="G118" s="36" t="s">
         <v>338</v>
       </c>
-      <c r="H118" s="54" t="s">
+      <c r="H118" s="53" t="s">
         <v>339</v>
       </c>
       <c r="I118" s="43" t="s">
@@ -9034,7 +9024,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="33" t="n">
         <v>156</v>
       </c>
@@ -9056,7 +9046,7 @@
       <c r="G119" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="H119" s="54" t="s">
+      <c r="H119" s="53" t="s">
         <v>345</v>
       </c>
       <c r="I119" s="44" t="s">
@@ -9097,7 +9087,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="33" t="n">
         <v>159</v>
       </c>
@@ -9119,7 +9109,7 @@
       <c r="G120" s="36" t="s">
         <v>350</v>
       </c>
-      <c r="H120" s="54" t="s">
+      <c r="H120" s="53" t="s">
         <v>351</v>
       </c>
       <c r="I120" s="44" t="s">
@@ -9138,7 +9128,7 @@
       <c r="N120" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O120" s="50" t="s">
+      <c r="O120" s="49" t="s">
         <v>353</v>
       </c>
       <c r="P120" s="37" t="s">
@@ -9160,7 +9150,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="33" t="n">
         <v>160</v>
       </c>
@@ -9182,7 +9172,7 @@
       <c r="G121" s="36" t="s">
         <v>357</v>
       </c>
-      <c r="H121" s="54" t="s">
+      <c r="H121" s="53" t="s">
         <v>358</v>
       </c>
       <c r="I121" s="44" t="s">
@@ -9223,7 +9213,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="344.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="33" t="n">
         <v>161</v>
       </c>
@@ -9245,7 +9235,7 @@
       <c r="G122" s="36" t="s">
         <v>364</v>
       </c>
-      <c r="H122" s="54" t="s">
+      <c r="H122" s="53" t="s">
         <v>365</v>
       </c>
       <c r="I122" s="44" t="s">
@@ -9264,7 +9254,7 @@
       <c r="N122" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O122" s="50" t="s">
+      <c r="O122" s="49" t="s">
         <v>367</v>
       </c>
       <c r="P122" s="37" t="s">
@@ -9286,7 +9276,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="33" t="n">
         <v>162</v>
       </c>
@@ -9308,7 +9298,7 @@
       <c r="G123" s="36" t="s">
         <v>371</v>
       </c>
-      <c r="H123" s="54" t="s">
+      <c r="H123" s="53" t="s">
         <v>372</v>
       </c>
       <c r="I123" s="44" t="s">
@@ -9347,7 +9337,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="33" t="n">
         <v>163</v>
       </c>
@@ -9369,7 +9359,7 @@
       <c r="G124" s="36" t="s">
         <v>378</v>
       </c>
-      <c r="H124" s="54" t="s">
+      <c r="H124" s="53" t="s">
         <v>379</v>
       </c>
       <c r="I124" s="44" t="s">
@@ -9410,7 +9400,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="33" t="n">
         <v>164</v>
       </c>
@@ -9428,7 +9418,7 @@
       </c>
       <c r="F125" s="36"/>
       <c r="G125" s="36"/>
-      <c r="H125" s="48"/>
+      <c r="H125" s="47"/>
       <c r="I125" s="42"/>
       <c r="J125" s="37" t="s">
         <v>63</v>
@@ -9451,7 +9441,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="33" t="n">
         <v>165</v>
       </c>
@@ -9469,7 +9459,7 @@
       </c>
       <c r="F126" s="36"/>
       <c r="G126" s="36"/>
-      <c r="H126" s="48"/>
+      <c r="H126" s="47"/>
       <c r="I126" s="42"/>
       <c r="J126" s="37" t="s">
         <v>63</v>
@@ -9492,7 +9482,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="33" t="n">
         <v>166</v>
       </c>
@@ -9510,7 +9500,7 @@
       </c>
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
-      <c r="H127" s="48"/>
+      <c r="H127" s="47"/>
       <c r="I127" s="42"/>
       <c r="J127" s="37" t="s">
         <v>63</v>
@@ -9533,7 +9523,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="33" t="n">
         <v>167</v>
       </c>
@@ -9551,10 +9541,14 @@
       </c>
       <c r="F128" s="36"/>
       <c r="G128" s="36"/>
-      <c r="H128" s="48"/>
+      <c r="H128" s="47"/>
       <c r="I128" s="42"/>
-      <c r="J128" s="37"/>
-      <c r="K128" s="37"/>
+      <c r="J128" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K128" s="37" t="s">
+        <v>383</v>
+      </c>
       <c r="L128" s="37"/>
       <c r="M128" s="37"/>
       <c r="N128" s="37"/>
@@ -9570,7 +9564,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="33" t="n">
         <v>168</v>
       </c>
@@ -9627,7 +9621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="33" t="n">
         <v>169</v>
       </c>
@@ -10985,7 +10979,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="33" t="n">
         <v>448</v>
       </c>
@@ -11032,7 +11026,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="33" t="n">
         <v>449</v>
       </c>
@@ -11079,7 +11073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="33" t="n">
         <v>450</v>
       </c>
@@ -11126,7 +11120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="33" t="n">
         <v>451</v>
       </c>
@@ -11473,7 +11467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="33" t="n">
         <v>461</v>
       </c>
@@ -11491,7 +11485,7 @@
       </c>
       <c r="F178" s="33"/>
       <c r="G178" s="33"/>
-      <c r="H178" s="55"/>
+      <c r="H178" s="54"/>
       <c r="I178" s="33"/>
       <c r="J178" s="37" t="s">
         <v>63</v>
@@ -11699,7 +11693,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="33" t="n">
         <v>467</v>
       </c>
@@ -11756,7 +11750,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="33" t="n">
         <v>468</v>
       </c>
@@ -12033,7 +12027,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="33" t="n">
         <v>475</v>
       </c>
@@ -12055,7 +12049,7 @@
       <c r="G192" s="36" t="s">
         <v>553</v>
       </c>
-      <c r="H192" s="52" t="s">
+      <c r="H192" s="51" t="s">
         <v>554</v>
       </c>
       <c r="I192" s="3" t="s">
@@ -16164,7 +16158,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="N169 I15"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16230,7 +16224,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="N169 A3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16245,7 +16239,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>563</v>
       </c>
       <c r="B1" s="20" t="s">
@@ -16257,158 +16251,158 @@
       <c r="D1" s="20" t="s">
         <v>565</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>566</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>569</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>571</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>573</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="61" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>575</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="60" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="59" t="s">
         <v>577</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="61" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="59" t="s">
         <v>579</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="61" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="59" t="s">
         <v>581</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="61" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="59" t="s">
         <v>583</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="61" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="s">
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="58" t="s">
         <v>585</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="62" t="s">
         <v>586</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="60" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="58" t="s">
         <v>568</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="59" t="s">
         <v>588</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="61" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="64"/>
+      <c r="D12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="64"/>
+      <c r="D13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -17378,7 +17372,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N169 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17389,32 +17383,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>590</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>591</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>